<commit_message>
created medication profiles for 2400 sections; created fsh/terminology directory structure
</commit_message>
<xml_diff>
--- a/docs/ValueSet-med-gvhd-prophylaxis-vs.xlsx
+++ b/docs/ValueSet-med-gvhd-prophylaxis-vs.xlsx
@@ -36,7 +36,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>RxNormGVHDProphylaxis</t>
+    <t>RxNormGVHDProphylaxisVS</t>
   </si>
   <si>
     <t>Title</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-08-09T17:12:26-05:00</t>
+    <t>2022-08-10T08:52:57-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>